<commit_message>
Updated Excel reading Process
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>bc_SelectAnEnvironment</t>
   </si>
@@ -45,12 +45,6 @@
     <t>bc_ClickOnExecute</t>
   </si>
   <si>
-    <t>vb</t>
-  </si>
-  <si>
-    <t>gfdgf</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
@@ -61,6 +55,51 @@
   </si>
   <si>
     <t>tc_LoginTest</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Loadt01</t>
+  </si>
+  <si>
+    <t>Loadt02</t>
+  </si>
+  <si>
+    <t>Loadt03</t>
+  </si>
+  <si>
+    <t>Loadt04</t>
+  </si>
+  <si>
+    <t>Loadt05</t>
+  </si>
+  <si>
+    <t>Loadt06</t>
+  </si>
+  <si>
+    <t>Loadt07</t>
+  </si>
+  <si>
+    <t>Loadt08</t>
+  </si>
+  <si>
+    <t>URL2</t>
+  </si>
+  <si>
+    <t>URL3</t>
+  </si>
+  <si>
+    <t>URL4</t>
+  </si>
+  <si>
+    <t>URL5</t>
+  </si>
+  <si>
+    <t>URL7</t>
+  </si>
+  <si>
+    <t>URL8</t>
   </si>
 </sst>
 </file>
@@ -430,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,92 +481,223 @@
     <col min="2" max="2" width="48.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://aenetworks.oktapreview.com/login/default"/>
+    <hyperlink ref="B5" r:id="rId2" display="https://aenetworks.oktapreview.com/login/default"/>
+    <hyperlink ref="B7" r:id="rId3" display="https://aenetworks.oktapreview.com/login/default"/>
+    <hyperlink ref="B6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:E16"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" t="s">
         <v>6</v>
       </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3:B9" r:id="rId2" display="https://aenetworks.oktapreview.com/login/default"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId1"/>
-  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated with static methods for business components
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="31">
   <si>
     <t>bc_SelectAnEnvironment</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -541,9 +544,6 @@
     <hyperlink ref="B2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId4"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -552,7 +552,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,9 +652,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId1"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -663,7 +660,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,8 +705,8 @@
       <c r="C3" t="s">
         <v>28</v>
       </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -769,9 +766,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId1"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -894,8 +888,5 @@
     <hyperlink ref="B3:B9" r:id="rId2" display="https://aenetworks.oktapreview.com/login/default"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId3"/>
-  </customProperties>
 </worksheet>
 </file>
</xml_diff>